<commit_message>
Messed up the column
</commit_message>
<xml_diff>
--- a/Exel_datasheet.xlsx
+++ b/Exel_datasheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Hugo/Documents/GitHub/Cancer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{867A568E-B967-FA4F-A9A5-55BC135EBD20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DF875A2-BAB0-0D4E-93F1-7DDC7248C0F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10940" yWindow="2080" windowWidth="28800" windowHeight="16560" xr2:uid="{3F2E20AE-210F-164C-8C08-0F2465EFFE5F}"/>
   </bookViews>
@@ -202,8 +202,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8916ECA0-BA80-584B-91DE-C69ADCF3C878}" name="Table1" displayName="Table1" ref="A1:B90" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3" tableBorderDxfId="2">
   <autoFilter ref="A1:B90" xr:uid="{8916ECA0-BA80-584B-91DE-C69ADCF3C878}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{F4C92C04-34DC-FA42-ACC2-1D83FC418E28}" name="H" dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{CD04C48C-F6F2-EA46-9100-986A13715296}" name="F" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{F4C92C04-34DC-FA42-ACC2-1D83FC418E28}" name="F" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{CD04C48C-F6F2-EA46-9100-986A13715296}" name="H" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -520,7 +520,7 @@
   <dimension ref="A1:J90"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -531,10 +531,10 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
       </c>
       <c r="H1" t="s">
         <v>2</v>

</xml_diff>

<commit_message>
gender specific cancer data
Error on line 17, needs to be fixed
</commit_message>
<xml_diff>
--- a/Exel_datasheet.xlsx
+++ b/Exel_datasheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Hugo/Documents/GitHub/Cancer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DF875A2-BAB0-0D4E-93F1-7DDC7248C0F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0AE2C83-3AF2-094A-8E7B-DE5A3B9748FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10940" yWindow="2080" windowWidth="28800" windowHeight="16560" xr2:uid="{3F2E20AE-210F-164C-8C08-0F2465EFFE5F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="3">
   <si>
     <t>F</t>
   </si>
@@ -44,10 +44,7 @@
     <t>H</t>
   </si>
   <si>
-    <t>Prostate_surv</t>
-  </si>
-  <si>
-    <t>Breast_surv</t>
+    <t>prostate/breast cancer rates:</t>
   </si>
 </sst>
 </file>
@@ -213,8 +210,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D0178F4F-7295-E741-9234-4B28B812C8DB}" name="Table3" displayName="Table3" ref="H1:I90" totalsRowShown="0">
   <autoFilter ref="H1:I90" xr:uid="{D0178F4F-7295-E741-9234-4B28B812C8DB}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{57040153-3BA2-784B-A6C4-693107988B5A}" name="Prostate_surv"/>
-    <tableColumn id="2" xr3:uid="{8A08188B-C4B6-1144-BA3A-0683AAA95122}" name="Breast_surv"/>
+    <tableColumn id="1" xr3:uid="{57040153-3BA2-784B-A6C4-693107988B5A}" name="H"/>
+    <tableColumn id="2" xr3:uid="{8A08188B-C4B6-1144-BA3A-0683AAA95122}" name="F"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -520,7 +517,7 @@
   <dimension ref="A1:J90"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -536,11 +533,14 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="G1" t="s">
+        <v>2</v>
+      </c>
       <c r="H1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I1" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Trying things with excel
</commit_message>
<xml_diff>
--- a/Exel_datasheet.xlsx
+++ b/Exel_datasheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Hugo/Documents/GitHub/Cancer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FD9B757-B90B-AA4B-98CF-24B4E31150DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DE8379A-CF13-CA40-98B9-41B7A3CCB993}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9600" yWindow="2080" windowWidth="28800" windowHeight="16560" xr2:uid="{3F2E20AE-210F-164C-8C08-0F2465EFFE5F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>F</t>
   </si>
@@ -44,13 +44,10 @@
     <t>H</t>
   </si>
   <si>
-    <t>prostate/breast cancer rates:</t>
-  </si>
-  <si>
     <t>H_canc</t>
   </si>
   <si>
-    <t>F_canc</t>
+    <t>Column2</t>
   </si>
 </sst>
 </file>
@@ -60,7 +57,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -71,6 +68,23 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF6F6F6F"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -95,17 +109,61 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="7">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF6F6F6F"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="#,##0.0"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color rgb="FF6F6F6F"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="#,##0.0"/>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -202,22 +260,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8916ECA0-BA80-584B-91DE-C69ADCF3C878}" name="Table1" displayName="Table1" ref="A1:B90" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3" tableBorderDxfId="2">
-  <autoFilter ref="A1:B90" xr:uid="{8916ECA0-BA80-584B-91DE-C69ADCF3C878}"/>
-  <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{F4C92C04-34DC-FA42-ACC2-1D83FC418E28}" name="F" dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{CD04C48C-F6F2-EA46-9100-986A13715296}" name="H" dataDxfId="0"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D0178F4F-7295-E741-9234-4B28B812C8DB}" name="Table3" displayName="Table3" ref="H1:I90" totalsRowShown="0">
-  <autoFilter ref="H1:I90" xr:uid="{D0178F4F-7295-E741-9234-4B28B812C8DB}"/>
-  <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{57040153-3BA2-784B-A6C4-693107988B5A}" name="H_canc"/>
-    <tableColumn id="2" xr3:uid="{8A08188B-C4B6-1144-BA3A-0683AAA95122}" name="F_canc"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8916ECA0-BA80-584B-91DE-C69ADCF3C878}" name="Table1" displayName="Table1" ref="A1:D90" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5" tableBorderDxfId="4">
+  <autoFilter ref="A1:D90" xr:uid="{8916ECA0-BA80-584B-91DE-C69ADCF3C878}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{F4C92C04-34DC-FA42-ACC2-1D83FC418E28}" name="F" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{CD04C48C-F6F2-EA46-9100-986A13715296}" name="H" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{57C64BBD-9ADD-CD45-956A-5CE6EDDD48D9}" name="H_canc" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{6B6BDBED-B8AF-CA42-8537-2544D6CD8FB0}" name="Column2" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -520,10 +569,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30632C49-4E9C-7241-AF43-E9927BC57264}">
-  <dimension ref="A1:J90"/>
+  <dimension ref="A1:H90"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -532,969 +581,1055 @@
     <col min="2" max="2" width="37.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="G1" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="H1" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="I1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1.8699999999999998E-2</v>
       </c>
       <c r="B2">
         <v>2.0899999999999998E-2</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="D2" s="3"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1.8699999999999998E-2</v>
       </c>
       <c r="B3">
         <v>2.0899999999999998E-2</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="D3" s="3"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1.8699999999999998E-2</v>
       </c>
       <c r="B4">
         <v>2.0899999999999998E-2</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="D4" s="3"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1.0199999999999999E-2</v>
       </c>
       <c r="B5">
         <v>1.1300000000000001E-2</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="D5" s="3"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1.0199999999999999E-2</v>
       </c>
       <c r="B6">
         <v>1.1300000000000001E-2</v>
       </c>
-      <c r="J6" s="2"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="D6" s="3"/>
+      <c r="H6" s="2"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1.0199999999999999E-2</v>
       </c>
       <c r="B7">
         <v>1.1300000000000001E-2</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="D7" s="3"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1.0199999999999999E-2</v>
       </c>
       <c r="B8">
         <v>1.1300000000000001E-2</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="D8" s="3"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1.0199999999999999E-2</v>
       </c>
       <c r="B9">
         <v>1.1300000000000001E-2</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="D9" s="3"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1.14E-2</v>
       </c>
       <c r="B10">
         <v>1.29E-2</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="D10" s="3"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>1.14E-2</v>
       </c>
       <c r="B11">
         <v>1.29E-2</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="D11" s="3"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>1.14E-2</v>
       </c>
       <c r="B12">
         <v>1.29E-2</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="D12" s="3"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>1.14E-2</v>
       </c>
       <c r="B13">
         <v>1.29E-2</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="D13" s="3"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>1.14E-2</v>
       </c>
       <c r="B14">
         <v>1.29E-2</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="D14" s="3"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>0.02</v>
       </c>
       <c r="B15">
         <v>1.9199999999999998E-2</v>
       </c>
-      <c r="H15">
-        <v>91.2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C15">
+        <v>91.2</v>
+      </c>
+      <c r="D15" s="3"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>0.02</v>
       </c>
       <c r="B16">
         <v>1.9199999999999998E-2</v>
       </c>
-      <c r="H16">
-        <v>91.2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C16">
+        <v>91.2</v>
+      </c>
+      <c r="D16" s="3"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>0.02</v>
       </c>
       <c r="B17">
         <v>1.9199999999999998E-2</v>
       </c>
-      <c r="H17">
-        <v>91.2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C17">
+        <v>91.2</v>
+      </c>
+      <c r="D17" s="3"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>0.02</v>
       </c>
       <c r="B18">
         <v>1.9199999999999998E-2</v>
       </c>
-      <c r="H18">
-        <v>91.2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C18">
+        <v>91.2</v>
+      </c>
+      <c r="D18" s="3"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>0.02</v>
       </c>
       <c r="B19">
         <v>1.9199999999999998E-2</v>
       </c>
-      <c r="H19">
-        <v>91.2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C19">
+        <v>91.2</v>
+      </c>
+      <c r="D19" s="3"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>3.3299999999999996E-2</v>
       </c>
       <c r="B20">
         <v>2.98E-2</v>
       </c>
-      <c r="H20">
-        <v>91.2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C20">
+        <v>91.2</v>
+      </c>
+      <c r="D20" s="3"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>3.3299999999999996E-2</v>
       </c>
       <c r="B21">
         <v>2.98E-2</v>
       </c>
-      <c r="H21">
-        <v>91.2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C21">
+        <v>91.2</v>
+      </c>
+      <c r="D21" s="3"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>3.3299999999999996E-2</v>
       </c>
       <c r="B22">
         <v>2.98E-2</v>
       </c>
-      <c r="H22">
-        <v>91.2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C22">
+        <v>91.2</v>
+      </c>
+      <c r="D22" s="3"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>3.3299999999999996E-2</v>
       </c>
       <c r="B23">
         <v>2.98E-2</v>
       </c>
-      <c r="H23">
-        <v>91.2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C23">
+        <v>91.2</v>
+      </c>
+      <c r="D23" s="3"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>3.3299999999999996E-2</v>
       </c>
       <c r="B24">
         <v>2.98E-2</v>
       </c>
-      <c r="H24">
-        <v>91.2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C24">
+        <v>91.2</v>
+      </c>
+      <c r="D24" s="3"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>7.2099999999999997E-2</v>
       </c>
       <c r="B25">
         <v>4.6399999999999997E-2</v>
       </c>
-      <c r="H25">
-        <v>91.2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C25">
+        <v>91.2</v>
+      </c>
+      <c r="D25" s="3"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>7.2099999999999997E-2</v>
       </c>
       <c r="B26">
         <v>4.6399999999999997E-2</v>
       </c>
-      <c r="H26">
-        <v>91.2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C26">
+        <v>91.2</v>
+      </c>
+      <c r="D26" s="3"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>7.2099999999999997E-2</v>
       </c>
       <c r="B27">
         <v>4.6399999999999997E-2</v>
       </c>
-      <c r="H27">
-        <v>91.2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C27">
+        <v>91.2</v>
+      </c>
+      <c r="D27" s="3"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>7.2099999999999997E-2</v>
       </c>
       <c r="B28">
         <v>4.6399999999999997E-2</v>
       </c>
-      <c r="H28">
-        <v>91.2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C28">
+        <v>91.2</v>
+      </c>
+      <c r="D28" s="3"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>7.2099999999999997E-2</v>
       </c>
       <c r="B29">
         <v>4.6399999999999997E-2</v>
       </c>
-      <c r="H29">
-        <v>91.2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C29">
+        <v>91.2</v>
+      </c>
+      <c r="D29" s="3"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>0.11749999999999999</v>
       </c>
       <c r="B30">
         <v>6.7699999999999996E-2</v>
       </c>
-      <c r="H30">
-        <v>91.2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C30">
+        <v>91.2</v>
+      </c>
+      <c r="D30" s="3"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>0.11749999999999999</v>
       </c>
       <c r="B31">
         <v>6.7699999999999996E-2</v>
       </c>
-      <c r="H31">
-        <v>91.2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C31">
+        <v>91.2</v>
+      </c>
+      <c r="D31" s="3"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>0.11749999999999999</v>
       </c>
       <c r="B32">
         <v>6.7699999999999996E-2</v>
       </c>
-      <c r="H32">
-        <v>91.2</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C32">
+        <v>91.2</v>
+      </c>
+      <c r="D32" s="3"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>0.11749999999999999</v>
       </c>
       <c r="B33">
         <v>6.7699999999999996E-2</v>
       </c>
-      <c r="H33">
-        <v>91.2</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C33">
+        <v>91.2</v>
+      </c>
+      <c r="D33" s="3"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>0.11749999999999999</v>
       </c>
       <c r="B34">
         <v>6.7699999999999996E-2</v>
       </c>
-      <c r="H34">
-        <v>91.2</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C34">
+        <v>91.2</v>
+      </c>
+      <c r="D34" s="3"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>0.1721</v>
       </c>
       <c r="B35">
         <v>8.8099999999999998E-2</v>
       </c>
-      <c r="H35">
-        <v>91.2</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C35">
+        <v>91.2</v>
+      </c>
+      <c r="D35" s="3"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>0.1721</v>
       </c>
       <c r="B36">
         <v>8.8099999999999998E-2</v>
       </c>
-      <c r="H36">
-        <v>91.2</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C36">
+        <v>91.2</v>
+      </c>
+      <c r="D36" s="3"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>0.1721</v>
       </c>
       <c r="B37">
         <v>8.8099999999999998E-2</v>
       </c>
-      <c r="H37">
-        <v>91.2</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C37">
+        <v>91.2</v>
+      </c>
+      <c r="D37" s="3"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>0.1721</v>
       </c>
       <c r="B38">
         <v>8.8099999999999998E-2</v>
       </c>
-      <c r="H38">
-        <v>91.2</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C38">
+        <v>91.2</v>
+      </c>
+      <c r="D38" s="3"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>0.1721</v>
       </c>
       <c r="B39">
         <v>8.8099999999999998E-2</v>
       </c>
-      <c r="H39">
-        <v>91.2</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C39">
+        <v>91.2</v>
+      </c>
+      <c r="D39" s="3"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>0.26330000000000003</v>
       </c>
       <c r="B40">
         <v>0.124</v>
       </c>
-      <c r="H40">
-        <v>91.2</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C40">
+        <v>91.2</v>
+      </c>
+      <c r="D40" s="3"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>0.26330000000000003</v>
       </c>
       <c r="B41">
         <v>0.124</v>
       </c>
-      <c r="H41">
-        <v>91.2</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C41">
+        <v>91.2</v>
+      </c>
+      <c r="D41" s="3"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>0.26330000000000003</v>
       </c>
       <c r="B42">
         <v>0.124</v>
       </c>
-      <c r="H42">
-        <v>91.2</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C42">
+        <v>91.2</v>
+      </c>
+      <c r="D42" s="3"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>0.26330000000000003</v>
       </c>
       <c r="B43">
         <v>0.124</v>
       </c>
-      <c r="H43">
-        <v>91.2</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C43">
+        <v>91.2</v>
+      </c>
+      <c r="D43" s="3"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>0.26330000000000003</v>
       </c>
       <c r="B44">
         <v>0.124</v>
       </c>
-      <c r="H44">
-        <v>91.2</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C44">
+        <v>91.2</v>
+      </c>
+      <c r="D44" s="3"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>0.41410000000000002</v>
       </c>
       <c r="B45">
         <v>0.21459999999999999</v>
       </c>
-      <c r="H45">
-        <v>91.2</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C45">
+        <v>91.2</v>
+      </c>
+      <c r="D45" s="3"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>0.41410000000000002</v>
       </c>
       <c r="B46">
         <v>0.21459999999999999</v>
       </c>
-      <c r="H46">
-        <v>91.2</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C46">
+        <v>91.2</v>
+      </c>
+      <c r="D46" s="3"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>0.41410000000000002</v>
       </c>
       <c r="B47">
         <v>0.21459999999999999</v>
       </c>
-      <c r="H47">
-        <v>91.2</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C47">
+        <v>91.2</v>
+      </c>
+      <c r="D47" s="3"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>0.41410000000000002</v>
       </c>
       <c r="B48">
         <v>0.21459999999999999</v>
       </c>
-      <c r="H48">
-        <v>91.2</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C48">
+        <v>91.2</v>
+      </c>
+      <c r="D48" s="3"/>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>0.41410000000000002</v>
       </c>
       <c r="B49">
         <v>0.21459999999999999</v>
       </c>
-      <c r="H49">
-        <v>91.2</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C49">
+        <v>91.2</v>
+      </c>
+      <c r="D49" s="3"/>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>0.57550000000000001</v>
       </c>
       <c r="B50">
         <v>0.39319999999999999</v>
       </c>
-      <c r="H50">
+      <c r="C50">
         <v>92.8</v>
       </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D50" s="3"/>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>0.57550000000000001</v>
       </c>
       <c r="B51">
         <v>0.39319999999999999</v>
       </c>
-      <c r="H51">
+      <c r="C51">
         <v>92.8</v>
       </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D51" s="3"/>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>0.57550000000000001</v>
       </c>
       <c r="B52">
         <v>0.39319999999999999</v>
       </c>
-      <c r="H52">
+      <c r="C52">
         <v>92.8</v>
       </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D52" s="3"/>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>0.57550000000000001</v>
       </c>
       <c r="B53">
         <v>0.39319999999999999</v>
       </c>
-      <c r="H53">
+      <c r="C53">
         <v>92.8</v>
       </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D53" s="3"/>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>0.57550000000000001</v>
       </c>
       <c r="B54">
         <v>0.39319999999999999</v>
       </c>
-      <c r="H54">
+      <c r="C54">
         <v>92.8</v>
       </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D54" s="3"/>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>0.73409999999999997</v>
       </c>
       <c r="B55">
         <v>0.71120000000000005</v>
       </c>
-      <c r="H55">
+      <c r="C55">
         <v>92.8</v>
       </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D55" s="3"/>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>0.73409999999999997</v>
       </c>
       <c r="B56">
         <v>0.71120000000000005</v>
       </c>
-      <c r="H56">
+      <c r="C56">
         <v>92.8</v>
       </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D56" s="3"/>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>0.73409999999999997</v>
       </c>
       <c r="B57">
         <v>0.71120000000000005</v>
       </c>
-      <c r="H57">
+      <c r="C57">
         <v>92.8</v>
       </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D57" s="3"/>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>0.73409999999999997</v>
       </c>
       <c r="B58">
         <v>0.71120000000000005</v>
       </c>
-      <c r="H58">
+      <c r="C58">
         <v>92.8</v>
       </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D58" s="3"/>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>0.73409999999999997</v>
       </c>
       <c r="B59">
         <v>0.71120000000000005</v>
       </c>
-      <c r="H59">
+      <c r="C59">
         <v>92.8</v>
       </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D59" s="3"/>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>0.97820000000000007</v>
       </c>
       <c r="B60">
         <v>1.1557999999999999</v>
       </c>
-      <c r="H60">
+      <c r="C60">
         <v>93.8</v>
       </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D60" s="3"/>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>0.97820000000000007</v>
       </c>
       <c r="B61">
         <v>1.1557999999999999</v>
       </c>
-      <c r="H61">
+      <c r="C61">
         <v>93.8</v>
       </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D61" s="3"/>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>0.97820000000000007</v>
       </c>
       <c r="B62">
         <v>1.1557999999999999</v>
       </c>
-      <c r="H62">
+      <c r="C62">
         <v>93.8</v>
       </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D62" s="3"/>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>0.97820000000000007</v>
       </c>
       <c r="B63">
         <v>1.1557999999999999</v>
       </c>
-      <c r="H63">
+      <c r="C63">
         <v>93.8</v>
       </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D63" s="3"/>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>0.97820000000000007</v>
       </c>
       <c r="B64">
         <v>1.1557999999999999</v>
       </c>
-      <c r="H64">
+      <c r="C64">
         <v>93.8</v>
       </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D64" s="3"/>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>1.2844</v>
       </c>
       <c r="B65">
         <v>1.7749000000000001</v>
       </c>
-      <c r="H65">
+      <c r="C65">
         <v>93.8</v>
       </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D65" s="3"/>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>1.2844</v>
       </c>
       <c r="B66">
         <v>1.7749000000000001</v>
       </c>
-      <c r="H66">
+      <c r="C66">
         <v>93.8</v>
       </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D66" s="3"/>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>1.2844</v>
       </c>
       <c r="B67">
         <v>1.7749000000000001</v>
       </c>
-      <c r="H67">
+      <c r="C67">
         <v>93.8</v>
       </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D67" s="3"/>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>1.2844</v>
       </c>
       <c r="B68">
         <v>1.7749000000000001</v>
       </c>
-      <c r="H68">
+      <c r="C68">
         <v>93.8</v>
       </c>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D68" s="3"/>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>1.2844</v>
       </c>
       <c r="B69">
         <v>1.7749000000000001</v>
       </c>
-      <c r="H69">
+      <c r="C69">
         <v>93.8</v>
       </c>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D69" s="3"/>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>1.5217000000000001</v>
       </c>
       <c r="B70">
         <v>2.3283</v>
       </c>
-      <c r="H70">
+      <c r="C70">
         <v>89.4</v>
       </c>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D70" s="3"/>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>1.5217000000000001</v>
       </c>
       <c r="B71">
         <v>2.3283</v>
       </c>
-      <c r="H71">
+      <c r="C71">
         <v>89.4</v>
       </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D71" s="3"/>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>1.5217000000000001</v>
       </c>
       <c r="B72">
         <v>2.3283</v>
       </c>
-      <c r="H72">
+      <c r="C72">
         <v>89.4</v>
       </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D72" s="3"/>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>1.5217000000000001</v>
       </c>
       <c r="B73">
         <v>2.3283</v>
       </c>
-      <c r="H73">
+      <c r="C73">
         <v>89.4</v>
       </c>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D73" s="3"/>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>1.5217000000000001</v>
       </c>
       <c r="B74">
         <v>2.3283</v>
       </c>
-      <c r="H74">
+      <c r="C74">
         <v>89.4</v>
       </c>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D74" s="3"/>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>1.8572</v>
       </c>
       <c r="B75">
         <v>2.9163000000000001</v>
       </c>
-      <c r="H75">
+      <c r="C75">
         <v>89.4</v>
       </c>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D75" s="3"/>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>1.8572</v>
       </c>
       <c r="B76">
         <v>2.9163000000000001</v>
       </c>
-      <c r="H76">
+      <c r="C76">
         <v>89.4</v>
       </c>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D76" s="3"/>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>1.8572</v>
       </c>
       <c r="B77">
         <v>2.9163000000000001</v>
       </c>
-      <c r="H77">
+      <c r="C77">
         <v>89.4</v>
       </c>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D77" s="3"/>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>1.8572</v>
       </c>
       <c r="B78">
         <v>2.9163000000000001</v>
       </c>
-      <c r="H78">
+      <c r="C78">
         <v>89.4</v>
       </c>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D78" s="3"/>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>1.8572</v>
       </c>
       <c r="B79">
         <v>2.9163000000000001</v>
       </c>
-      <c r="H79">
+      <c r="C79">
         <v>89.4</v>
       </c>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D79" s="3"/>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>2.0796999999999999</v>
       </c>
       <c r="B80">
         <v>3.1324999999999998</v>
       </c>
-      <c r="H80">
+      <c r="C80">
         <v>65.7</v>
       </c>
-    </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D80" s="3"/>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>2.0796999999999999</v>
       </c>
       <c r="B81">
         <v>3.1324999999999998</v>
       </c>
-      <c r="H81">
+      <c r="C81">
         <v>65.7</v>
       </c>
-    </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D81" s="3"/>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>2.0796999999999999</v>
       </c>
       <c r="B82">
         <v>3.1324999999999998</v>
       </c>
-      <c r="H82">
+      <c r="C82">
         <v>65.7</v>
       </c>
-    </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D82" s="3"/>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>2.0796999999999999</v>
       </c>
       <c r="B83">
         <v>3.1324999999999998</v>
       </c>
-      <c r="H83">
+      <c r="C83">
         <v>65.7</v>
       </c>
-    </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D83" s="3"/>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>2.0796999999999999</v>
       </c>
       <c r="B84">
         <v>3.1324999999999998</v>
       </c>
-      <c r="H84">
+      <c r="C84">
         <v>65.7</v>
       </c>
-    </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D84" s="3"/>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>2.2229000000000001</v>
       </c>
       <c r="B85">
         <v>3.4116</v>
       </c>
-      <c r="H85">
+      <c r="C85">
         <v>65.7</v>
       </c>
-    </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D85" s="3"/>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>2.2229000000000001</v>
       </c>
       <c r="B86">
         <v>3.4116</v>
       </c>
-      <c r="H86">
+      <c r="C86">
         <v>65.7</v>
       </c>
-    </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D86" s="3"/>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>2.2229000000000001</v>
       </c>
       <c r="B87">
         <v>3.4116</v>
       </c>
-      <c r="H87">
+      <c r="C87">
         <v>65.7</v>
       </c>
-    </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D87" s="3"/>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>2.2229000000000001</v>
       </c>
       <c r="B88">
         <v>3.4116</v>
       </c>
-      <c r="H88">
+      <c r="C88">
         <v>65.7</v>
       </c>
-    </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D88" s="3"/>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>2.2229000000000001</v>
       </c>
       <c r="B89">
         <v>3.4116</v>
       </c>
-      <c r="H89">
+      <c r="C89">
         <v>65.7</v>
       </c>
-    </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D89" s="3"/>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>1.9990999999999999</v>
       </c>
       <c r="B90">
         <v>3.2862</v>
       </c>
-      <c r="H90">
+      <c r="C90">
         <v>65.7</v>
       </c>
+      <c r="D90" s="3"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="2">
+  <tableParts count="1">
     <tablePart r:id="rId1"/>
-    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Finally made the focken thing work
Now indicates survival rates of the most common types of cancer for the given sex and age
</commit_message>
<xml_diff>
--- a/Exel_datasheet.xlsx
+++ b/Exel_datasheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Hugo/Documents/GitHub/Cancer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DE8379A-CF13-CA40-98B9-41B7A3CCB993}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBB26067-B3AB-B445-92FD-A972A3EE685D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9600" yWindow="2080" windowWidth="28800" windowHeight="16560" xr2:uid="{3F2E20AE-210F-164C-8C08-0F2465EFFE5F}"/>
   </bookViews>
@@ -571,8 +571,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30632C49-4E9C-7241-AF43-E9927BC57264}">
   <dimension ref="A1:H90"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
+      <selection activeCell="F89" sqref="F89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -723,7 +723,9 @@
       <c r="C15">
         <v>91.2</v>
       </c>
-      <c r="D15" s="3"/>
+      <c r="D15" s="3">
+        <v>84.9</v>
+      </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16">
@@ -735,7 +737,9 @@
       <c r="C16">
         <v>91.2</v>
       </c>
-      <c r="D16" s="3"/>
+      <c r="D16" s="3">
+        <v>84.9</v>
+      </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17">
@@ -747,7 +751,9 @@
       <c r="C17">
         <v>91.2</v>
       </c>
-      <c r="D17" s="3"/>
+      <c r="D17" s="3">
+        <v>84.9</v>
+      </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18">
@@ -759,7 +765,9 @@
       <c r="C18">
         <v>91.2</v>
       </c>
-      <c r="D18" s="3"/>
+      <c r="D18" s="3">
+        <v>84.9</v>
+      </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19">
@@ -771,7 +779,9 @@
       <c r="C19">
         <v>91.2</v>
       </c>
-      <c r="D19" s="3"/>
+      <c r="D19" s="3">
+        <v>84.9</v>
+      </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20">
@@ -783,7 +793,9 @@
       <c r="C20">
         <v>91.2</v>
       </c>
-      <c r="D20" s="3"/>
+      <c r="D20" s="3">
+        <v>84.9</v>
+      </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21">
@@ -795,7 +807,9 @@
       <c r="C21">
         <v>91.2</v>
       </c>
-      <c r="D21" s="3"/>
+      <c r="D21" s="3">
+        <v>84.9</v>
+      </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22">
@@ -807,7 +821,9 @@
       <c r="C22">
         <v>91.2</v>
       </c>
-      <c r="D22" s="3"/>
+      <c r="D22" s="3">
+        <v>84.9</v>
+      </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23">
@@ -819,7 +835,9 @@
       <c r="C23">
         <v>91.2</v>
       </c>
-      <c r="D23" s="3"/>
+      <c r="D23" s="3">
+        <v>84.9</v>
+      </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24">
@@ -831,7 +849,9 @@
       <c r="C24">
         <v>91.2</v>
       </c>
-      <c r="D24" s="3"/>
+      <c r="D24" s="3">
+        <v>84.9</v>
+      </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25">
@@ -843,7 +863,9 @@
       <c r="C25">
         <v>91.2</v>
       </c>
-      <c r="D25" s="3"/>
+      <c r="D25" s="3">
+        <v>84.9</v>
+      </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26">
@@ -855,7 +877,9 @@
       <c r="C26">
         <v>91.2</v>
       </c>
-      <c r="D26" s="3"/>
+      <c r="D26" s="3">
+        <v>84.9</v>
+      </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27">
@@ -867,7 +891,9 @@
       <c r="C27">
         <v>91.2</v>
       </c>
-      <c r="D27" s="3"/>
+      <c r="D27" s="3">
+        <v>84.9</v>
+      </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28">
@@ -879,7 +905,9 @@
       <c r="C28">
         <v>91.2</v>
       </c>
-      <c r="D28" s="3"/>
+      <c r="D28" s="3">
+        <v>84.9</v>
+      </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29">
@@ -891,7 +919,9 @@
       <c r="C29">
         <v>91.2</v>
       </c>
-      <c r="D29" s="3"/>
+      <c r="D29" s="3">
+        <v>84.9</v>
+      </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30">
@@ -903,7 +933,9 @@
       <c r="C30">
         <v>91.2</v>
       </c>
-      <c r="D30" s="3"/>
+      <c r="D30" s="3">
+        <v>84.9</v>
+      </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31">
@@ -915,7 +947,9 @@
       <c r="C31">
         <v>91.2</v>
       </c>
-      <c r="D31" s="3"/>
+      <c r="D31" s="3">
+        <v>84.9</v>
+      </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32">
@@ -927,7 +961,9 @@
       <c r="C32">
         <v>91.2</v>
       </c>
-      <c r="D32" s="3"/>
+      <c r="D32" s="3">
+        <v>84.9</v>
+      </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33">
@@ -939,7 +975,9 @@
       <c r="C33">
         <v>91.2</v>
       </c>
-      <c r="D33" s="3"/>
+      <c r="D33" s="3">
+        <v>84.9</v>
+      </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34">
@@ -951,7 +989,9 @@
       <c r="C34">
         <v>91.2</v>
       </c>
-      <c r="D34" s="3"/>
+      <c r="D34" s="3">
+        <v>84.9</v>
+      </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35">
@@ -963,7 +1003,9 @@
       <c r="C35">
         <v>91.2</v>
       </c>
-      <c r="D35" s="3"/>
+      <c r="D35" s="3">
+        <v>84.9</v>
+      </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36">
@@ -975,7 +1017,9 @@
       <c r="C36">
         <v>91.2</v>
       </c>
-      <c r="D36" s="3"/>
+      <c r="D36" s="3">
+        <v>84.9</v>
+      </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37">
@@ -987,7 +1031,9 @@
       <c r="C37">
         <v>91.2</v>
       </c>
-      <c r="D37" s="3"/>
+      <c r="D37" s="3">
+        <v>84.9</v>
+      </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38">
@@ -999,7 +1045,9 @@
       <c r="C38">
         <v>91.2</v>
       </c>
-      <c r="D38" s="3"/>
+      <c r="D38" s="3">
+        <v>84.9</v>
+      </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39">
@@ -1011,7 +1059,9 @@
       <c r="C39">
         <v>91.2</v>
       </c>
-      <c r="D39" s="3"/>
+      <c r="D39" s="3">
+        <v>84.9</v>
+      </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40">
@@ -1023,7 +1073,9 @@
       <c r="C40">
         <v>91.2</v>
       </c>
-      <c r="D40" s="3"/>
+      <c r="D40" s="3">
+        <v>90</v>
+      </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41">
@@ -1035,7 +1087,9 @@
       <c r="C41">
         <v>91.2</v>
       </c>
-      <c r="D41" s="3"/>
+      <c r="D41" s="3">
+        <v>90</v>
+      </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42">
@@ -1047,7 +1101,9 @@
       <c r="C42">
         <v>91.2</v>
       </c>
-      <c r="D42" s="3"/>
+      <c r="D42" s="3">
+        <v>90</v>
+      </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43">
@@ -1059,7 +1115,9 @@
       <c r="C43">
         <v>91.2</v>
       </c>
-      <c r="D43" s="3"/>
+      <c r="D43" s="3">
+        <v>90</v>
+      </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44">
@@ -1071,7 +1129,9 @@
       <c r="C44">
         <v>91.2</v>
       </c>
-      <c r="D44" s="3"/>
+      <c r="D44" s="3">
+        <v>90</v>
+      </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45">
@@ -1083,7 +1143,9 @@
       <c r="C45">
         <v>91.2</v>
       </c>
-      <c r="D45" s="3"/>
+      <c r="D45" s="3">
+        <v>90</v>
+      </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46">
@@ -1095,7 +1157,9 @@
       <c r="C46">
         <v>91.2</v>
       </c>
-      <c r="D46" s="3"/>
+      <c r="D46" s="3">
+        <v>90</v>
+      </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47">
@@ -1107,7 +1171,9 @@
       <c r="C47">
         <v>91.2</v>
       </c>
-      <c r="D47" s="3"/>
+      <c r="D47" s="3">
+        <v>90</v>
+      </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48">
@@ -1119,7 +1185,9 @@
       <c r="C48">
         <v>91.2</v>
       </c>
-      <c r="D48" s="3"/>
+      <c r="D48" s="3">
+        <v>90</v>
+      </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49">
@@ -1131,7 +1199,9 @@
       <c r="C49">
         <v>91.2</v>
       </c>
-      <c r="D49" s="3"/>
+      <c r="D49" s="3">
+        <v>90</v>
+      </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50">
@@ -1143,7 +1213,9 @@
       <c r="C50">
         <v>92.8</v>
       </c>
-      <c r="D50" s="3"/>
+      <c r="D50" s="3">
+        <v>91.2</v>
+      </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51">
@@ -1155,7 +1227,9 @@
       <c r="C51">
         <v>92.8</v>
       </c>
-      <c r="D51" s="3"/>
+      <c r="D51" s="3">
+        <v>91.2</v>
+      </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52">
@@ -1167,7 +1241,9 @@
       <c r="C52">
         <v>92.8</v>
       </c>
-      <c r="D52" s="3"/>
+      <c r="D52" s="3">
+        <v>91.2</v>
+      </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53">
@@ -1179,7 +1255,9 @@
       <c r="C53">
         <v>92.8</v>
       </c>
-      <c r="D53" s="3"/>
+      <c r="D53" s="3">
+        <v>91.2</v>
+      </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54">
@@ -1191,7 +1269,9 @@
       <c r="C54">
         <v>92.8</v>
       </c>
-      <c r="D54" s="3"/>
+      <c r="D54" s="3">
+        <v>91.2</v>
+      </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55">
@@ -1203,7 +1283,9 @@
       <c r="C55">
         <v>92.8</v>
       </c>
-      <c r="D55" s="3"/>
+      <c r="D55" s="3">
+        <v>91.2</v>
+      </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56">
@@ -1215,7 +1297,9 @@
       <c r="C56">
         <v>92.8</v>
       </c>
-      <c r="D56" s="3"/>
+      <c r="D56" s="3">
+        <v>91.2</v>
+      </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57">
@@ -1227,7 +1311,9 @@
       <c r="C57">
         <v>92.8</v>
       </c>
-      <c r="D57" s="3"/>
+      <c r="D57" s="3">
+        <v>91.2</v>
+      </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58">
@@ -1239,7 +1325,9 @@
       <c r="C58">
         <v>92.8</v>
       </c>
-      <c r="D58" s="3"/>
+      <c r="D58" s="3">
+        <v>91.2</v>
+      </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59">
@@ -1251,7 +1339,9 @@
       <c r="C59">
         <v>92.8</v>
       </c>
-      <c r="D59" s="3"/>
+      <c r="D59" s="3">
+        <v>91.2</v>
+      </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60">
@@ -1263,7 +1353,9 @@
       <c r="C60">
         <v>93.8</v>
       </c>
-      <c r="D60" s="3"/>
+      <c r="D60" s="3">
+        <v>92.4</v>
+      </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61">
@@ -1275,7 +1367,9 @@
       <c r="C61">
         <v>93.8</v>
       </c>
-      <c r="D61" s="3"/>
+      <c r="D61" s="3">
+        <v>92.4</v>
+      </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62">
@@ -1287,7 +1381,9 @@
       <c r="C62">
         <v>93.8</v>
       </c>
-      <c r="D62" s="3"/>
+      <c r="D62" s="3">
+        <v>92.4</v>
+      </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63">
@@ -1299,7 +1395,9 @@
       <c r="C63">
         <v>93.8</v>
       </c>
-      <c r="D63" s="3"/>
+      <c r="D63" s="3">
+        <v>92.4</v>
+      </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64">
@@ -1311,7 +1409,9 @@
       <c r="C64">
         <v>93.8</v>
       </c>
-      <c r="D64" s="3"/>
+      <c r="D64" s="3">
+        <v>92.4</v>
+      </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65">
@@ -1323,7 +1423,9 @@
       <c r="C65">
         <v>93.8</v>
       </c>
-      <c r="D65" s="3"/>
+      <c r="D65" s="3">
+        <v>92.4</v>
+      </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A66">
@@ -1335,7 +1437,9 @@
       <c r="C66">
         <v>93.8</v>
       </c>
-      <c r="D66" s="3"/>
+      <c r="D66" s="3">
+        <v>92.4</v>
+      </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67">
@@ -1347,7 +1451,9 @@
       <c r="C67">
         <v>93.8</v>
       </c>
-      <c r="D67" s="3"/>
+      <c r="D67" s="3">
+        <v>92.4</v>
+      </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68">
@@ -1359,7 +1465,9 @@
       <c r="C68">
         <v>93.8</v>
       </c>
-      <c r="D68" s="3"/>
+      <c r="D68" s="3">
+        <v>92.4</v>
+      </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69">
@@ -1371,7 +1479,9 @@
       <c r="C69">
         <v>93.8</v>
       </c>
-      <c r="D69" s="3"/>
+      <c r="D69" s="3">
+        <v>92.4</v>
+      </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70">
@@ -1383,7 +1493,9 @@
       <c r="C70">
         <v>89.4</v>
       </c>
-      <c r="D70" s="3"/>
+      <c r="D70" s="3">
+        <v>83</v>
+      </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71">
@@ -1395,7 +1507,9 @@
       <c r="C71">
         <v>89.4</v>
       </c>
-      <c r="D71" s="3"/>
+      <c r="D71" s="3">
+        <v>83</v>
+      </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72">
@@ -1407,7 +1521,9 @@
       <c r="C72">
         <v>89.4</v>
       </c>
-      <c r="D72" s="3"/>
+      <c r="D72" s="3">
+        <v>83</v>
+      </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73">
@@ -1419,7 +1535,9 @@
       <c r="C73">
         <v>89.4</v>
       </c>
-      <c r="D73" s="3"/>
+      <c r="D73" s="3">
+        <v>83</v>
+      </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74">
@@ -1431,7 +1549,9 @@
       <c r="C74">
         <v>89.4</v>
       </c>
-      <c r="D74" s="3"/>
+      <c r="D74" s="3">
+        <v>83</v>
+      </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A75">
@@ -1443,7 +1563,9 @@
       <c r="C75">
         <v>89.4</v>
       </c>
-      <c r="D75" s="3"/>
+      <c r="D75" s="3">
+        <v>83</v>
+      </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A76">
@@ -1455,7 +1577,9 @@
       <c r="C76">
         <v>89.4</v>
       </c>
-      <c r="D76" s="3"/>
+      <c r="D76" s="3">
+        <v>83</v>
+      </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77">
@@ -1467,7 +1591,9 @@
       <c r="C77">
         <v>89.4</v>
       </c>
-      <c r="D77" s="3"/>
+      <c r="D77" s="3">
+        <v>83</v>
+      </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A78">
@@ -1479,7 +1605,9 @@
       <c r="C78">
         <v>89.4</v>
       </c>
-      <c r="D78" s="3"/>
+      <c r="D78" s="3">
+        <v>83</v>
+      </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A79">
@@ -1491,7 +1619,9 @@
       <c r="C79">
         <v>89.4</v>
       </c>
-      <c r="D79" s="3"/>
+      <c r="D79" s="3">
+        <v>83</v>
+      </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A80">
@@ -1503,7 +1633,9 @@
       <c r="C80">
         <v>65.7</v>
       </c>
-      <c r="D80" s="3"/>
+      <c r="D80" s="3">
+        <v>70.3</v>
+      </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A81">
@@ -1515,7 +1647,9 @@
       <c r="C81">
         <v>65.7</v>
       </c>
-      <c r="D81" s="3"/>
+      <c r="D81" s="3">
+        <v>70.3</v>
+      </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A82">
@@ -1527,7 +1661,9 @@
       <c r="C82">
         <v>65.7</v>
       </c>
-      <c r="D82" s="3"/>
+      <c r="D82" s="3">
+        <v>70.3</v>
+      </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83">
@@ -1539,7 +1675,9 @@
       <c r="C83">
         <v>65.7</v>
       </c>
-      <c r="D83" s="3"/>
+      <c r="D83" s="3">
+        <v>70.3</v>
+      </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A84">
@@ -1551,7 +1689,9 @@
       <c r="C84">
         <v>65.7</v>
       </c>
-      <c r="D84" s="3"/>
+      <c r="D84" s="3">
+        <v>70.3</v>
+      </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A85">
@@ -1563,7 +1703,9 @@
       <c r="C85">
         <v>65.7</v>
       </c>
-      <c r="D85" s="3"/>
+      <c r="D85" s="3">
+        <v>70.3</v>
+      </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A86">
@@ -1575,7 +1717,9 @@
       <c r="C86">
         <v>65.7</v>
       </c>
-      <c r="D86" s="3"/>
+      <c r="D86" s="3">
+        <v>70.3</v>
+      </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A87">
@@ -1587,7 +1731,9 @@
       <c r="C87">
         <v>65.7</v>
       </c>
-      <c r="D87" s="3"/>
+      <c r="D87" s="3">
+        <v>70.3</v>
+      </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A88">
@@ -1599,7 +1745,9 @@
       <c r="C88">
         <v>65.7</v>
       </c>
-      <c r="D88" s="3"/>
+      <c r="D88" s="3">
+        <v>70.3</v>
+      </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A89">
@@ -1611,7 +1759,9 @@
       <c r="C89">
         <v>65.7</v>
       </c>
-      <c r="D89" s="3"/>
+      <c r="D89" s="3">
+        <v>70.3</v>
+      </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90">
@@ -1623,7 +1773,9 @@
       <c r="C90">
         <v>65.7</v>
       </c>
-      <c r="D90" s="3"/>
+      <c r="D90" s="3">
+        <v>70.3</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
oopsie small mistake in column naming
</commit_message>
<xml_diff>
--- a/Exel_datasheet.xlsx
+++ b/Exel_datasheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Hugo/Documents/GitHub/Cancer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBB26067-B3AB-B445-92FD-A972A3EE685D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6D81917-13AE-E845-AA25-E7816B380F18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9600" yWindow="2080" windowWidth="28800" windowHeight="16560" xr2:uid="{3F2E20AE-210F-164C-8C08-0F2465EFFE5F}"/>
   </bookViews>
@@ -47,7 +47,7 @@
     <t>H_canc</t>
   </si>
   <si>
-    <t>Column2</t>
+    <t>F_canc</t>
   </si>
 </sst>
 </file>
@@ -266,7 +266,7 @@
     <tableColumn id="1" xr3:uid="{F4C92C04-34DC-FA42-ACC2-1D83FC418E28}" name="F" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{CD04C48C-F6F2-EA46-9100-986A13715296}" name="H" dataDxfId="2"/>
     <tableColumn id="3" xr3:uid="{57C64BBD-9ADD-CD45-956A-5CE6EDDD48D9}" name="H_canc" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{6B6BDBED-B8AF-CA42-8537-2544D6CD8FB0}" name="Column2" dataDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{6B6BDBED-B8AF-CA42-8537-2544D6CD8FB0}" name="F_canc" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -571,8 +571,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30632C49-4E9C-7241-AF43-E9927BC57264}">
   <dimension ref="A1:H90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
-      <selection activeCell="F89" sqref="F89"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
come on please work
</commit_message>
<xml_diff>
--- a/Exel_datasheet.xlsx
+++ b/Exel_datasheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Hugo/Documents/GitHub/Cancer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6D81917-13AE-E845-AA25-E7816B380F18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96D0079E-A3DA-6F49-9EB8-A17BF536DFCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9600" yWindow="2080" windowWidth="28800" windowHeight="16560" xr2:uid="{3F2E20AE-210F-164C-8C08-0F2465EFFE5F}"/>
   </bookViews>
@@ -57,7 +57,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -88,6 +88,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -109,7 +115,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -119,6 +125,9 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -572,7 +581,7 @@
   <dimension ref="A1:H90"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -723,7 +732,7 @@
       <c r="C15">
         <v>91.2</v>
       </c>
-      <c r="D15" s="3">
+      <c r="D15" s="5">
         <v>84.9</v>
       </c>
     </row>
@@ -737,7 +746,7 @@
       <c r="C16">
         <v>91.2</v>
       </c>
-      <c r="D16" s="3">
+      <c r="D16" s="5">
         <v>84.9</v>
       </c>
     </row>
@@ -751,7 +760,7 @@
       <c r="C17">
         <v>91.2</v>
       </c>
-      <c r="D17" s="3">
+      <c r="D17" s="5">
         <v>84.9</v>
       </c>
     </row>
@@ -765,7 +774,7 @@
       <c r="C18">
         <v>91.2</v>
       </c>
-      <c r="D18" s="3">
+      <c r="D18" s="5">
         <v>84.9</v>
       </c>
     </row>
@@ -779,7 +788,7 @@
       <c r="C19">
         <v>91.2</v>
       </c>
-      <c r="D19" s="3">
+      <c r="D19" s="5">
         <v>84.9</v>
       </c>
     </row>
@@ -793,7 +802,7 @@
       <c r="C20">
         <v>91.2</v>
       </c>
-      <c r="D20" s="3">
+      <c r="D20" s="5">
         <v>84.9</v>
       </c>
     </row>
@@ -807,7 +816,7 @@
       <c r="C21">
         <v>91.2</v>
       </c>
-      <c r="D21" s="3">
+      <c r="D21" s="5">
         <v>84.9</v>
       </c>
     </row>
@@ -821,7 +830,7 @@
       <c r="C22">
         <v>91.2</v>
       </c>
-      <c r="D22" s="3">
+      <c r="D22" s="5">
         <v>84.9</v>
       </c>
     </row>
@@ -835,7 +844,7 @@
       <c r="C23">
         <v>91.2</v>
       </c>
-      <c r="D23" s="3">
+      <c r="D23" s="5">
         <v>84.9</v>
       </c>
     </row>
@@ -849,7 +858,7 @@
       <c r="C24">
         <v>91.2</v>
       </c>
-      <c r="D24" s="3">
+      <c r="D24" s="5">
         <v>84.9</v>
       </c>
     </row>
@@ -863,7 +872,7 @@
       <c r="C25">
         <v>91.2</v>
       </c>
-      <c r="D25" s="3">
+      <c r="D25" s="5">
         <v>84.9</v>
       </c>
     </row>
@@ -877,7 +886,7 @@
       <c r="C26">
         <v>91.2</v>
       </c>
-      <c r="D26" s="3">
+      <c r="D26" s="5">
         <v>84.9</v>
       </c>
     </row>
@@ -891,7 +900,7 @@
       <c r="C27">
         <v>91.2</v>
       </c>
-      <c r="D27" s="3">
+      <c r="D27" s="5">
         <v>84.9</v>
       </c>
     </row>
@@ -905,7 +914,7 @@
       <c r="C28">
         <v>91.2</v>
       </c>
-      <c r="D28" s="3">
+      <c r="D28" s="5">
         <v>84.9</v>
       </c>
     </row>
@@ -919,7 +928,7 @@
       <c r="C29">
         <v>91.2</v>
       </c>
-      <c r="D29" s="3">
+      <c r="D29" s="5">
         <v>84.9</v>
       </c>
     </row>
@@ -933,7 +942,7 @@
       <c r="C30">
         <v>91.2</v>
       </c>
-      <c r="D30" s="3">
+      <c r="D30" s="5">
         <v>84.9</v>
       </c>
     </row>
@@ -947,7 +956,7 @@
       <c r="C31">
         <v>91.2</v>
       </c>
-      <c r="D31" s="3">
+      <c r="D31" s="5">
         <v>84.9</v>
       </c>
     </row>
@@ -961,7 +970,7 @@
       <c r="C32">
         <v>91.2</v>
       </c>
-      <c r="D32" s="3">
+      <c r="D32" s="5">
         <v>84.9</v>
       </c>
     </row>
@@ -975,7 +984,7 @@
       <c r="C33">
         <v>91.2</v>
       </c>
-      <c r="D33" s="3">
+      <c r="D33" s="5">
         <v>84.9</v>
       </c>
     </row>
@@ -989,7 +998,7 @@
       <c r="C34">
         <v>91.2</v>
       </c>
-      <c r="D34" s="3">
+      <c r="D34" s="5">
         <v>84.9</v>
       </c>
     </row>
@@ -1003,7 +1012,7 @@
       <c r="C35">
         <v>91.2</v>
       </c>
-      <c r="D35" s="3">
+      <c r="D35" s="5">
         <v>84.9</v>
       </c>
     </row>
@@ -1017,7 +1026,7 @@
       <c r="C36">
         <v>91.2</v>
       </c>
-      <c r="D36" s="3">
+      <c r="D36" s="5">
         <v>84.9</v>
       </c>
     </row>
@@ -1031,7 +1040,7 @@
       <c r="C37">
         <v>91.2</v>
       </c>
-      <c r="D37" s="3">
+      <c r="D37" s="5">
         <v>84.9</v>
       </c>
     </row>
@@ -1045,7 +1054,7 @@
       <c r="C38">
         <v>91.2</v>
       </c>
-      <c r="D38" s="3">
+      <c r="D38" s="5">
         <v>84.9</v>
       </c>
     </row>
@@ -1059,7 +1068,7 @@
       <c r="C39">
         <v>91.2</v>
       </c>
-      <c r="D39" s="3">
+      <c r="D39" s="5">
         <v>84.9</v>
       </c>
     </row>
@@ -1073,7 +1082,7 @@
       <c r="C40">
         <v>91.2</v>
       </c>
-      <c r="D40" s="3">
+      <c r="D40" s="5">
         <v>90</v>
       </c>
     </row>
@@ -1087,7 +1096,7 @@
       <c r="C41">
         <v>91.2</v>
       </c>
-      <c r="D41" s="3">
+      <c r="D41" s="5">
         <v>90</v>
       </c>
     </row>
@@ -1101,7 +1110,7 @@
       <c r="C42">
         <v>91.2</v>
       </c>
-      <c r="D42" s="3">
+      <c r="D42" s="5">
         <v>90</v>
       </c>
     </row>
@@ -1115,7 +1124,7 @@
       <c r="C43">
         <v>91.2</v>
       </c>
-      <c r="D43" s="3">
+      <c r="D43" s="5">
         <v>90</v>
       </c>
     </row>
@@ -1129,7 +1138,7 @@
       <c r="C44">
         <v>91.2</v>
       </c>
-      <c r="D44" s="3">
+      <c r="D44" s="5">
         <v>90</v>
       </c>
     </row>
@@ -1143,7 +1152,7 @@
       <c r="C45">
         <v>91.2</v>
       </c>
-      <c r="D45" s="3">
+      <c r="D45" s="5">
         <v>90</v>
       </c>
     </row>
@@ -1157,7 +1166,7 @@
       <c r="C46">
         <v>91.2</v>
       </c>
-      <c r="D46" s="3">
+      <c r="D46" s="5">
         <v>90</v>
       </c>
     </row>
@@ -1171,7 +1180,7 @@
       <c r="C47">
         <v>91.2</v>
       </c>
-      <c r="D47" s="3">
+      <c r="D47" s="5">
         <v>90</v>
       </c>
     </row>
@@ -1185,7 +1194,7 @@
       <c r="C48">
         <v>91.2</v>
       </c>
-      <c r="D48" s="3">
+      <c r="D48" s="5">
         <v>90</v>
       </c>
     </row>
@@ -1199,7 +1208,7 @@
       <c r="C49">
         <v>91.2</v>
       </c>
-      <c r="D49" s="3">
+      <c r="D49" s="5">
         <v>90</v>
       </c>
     </row>
@@ -1213,7 +1222,7 @@
       <c r="C50">
         <v>92.8</v>
       </c>
-      <c r="D50" s="3">
+      <c r="D50" s="5">
         <v>91.2</v>
       </c>
     </row>
@@ -1227,7 +1236,7 @@
       <c r="C51">
         <v>92.8</v>
       </c>
-      <c r="D51" s="3">
+      <c r="D51" s="5">
         <v>91.2</v>
       </c>
     </row>
@@ -1241,7 +1250,7 @@
       <c r="C52">
         <v>92.8</v>
       </c>
-      <c r="D52" s="3">
+      <c r="D52" s="5">
         <v>91.2</v>
       </c>
     </row>
@@ -1255,7 +1264,7 @@
       <c r="C53">
         <v>92.8</v>
       </c>
-      <c r="D53" s="3">
+      <c r="D53" s="5">
         <v>91.2</v>
       </c>
     </row>
@@ -1269,7 +1278,7 @@
       <c r="C54">
         <v>92.8</v>
       </c>
-      <c r="D54" s="3">
+      <c r="D54" s="5">
         <v>91.2</v>
       </c>
     </row>
@@ -1283,7 +1292,7 @@
       <c r="C55">
         <v>92.8</v>
       </c>
-      <c r="D55" s="3">
+      <c r="D55" s="5">
         <v>91.2</v>
       </c>
     </row>
@@ -1297,7 +1306,7 @@
       <c r="C56">
         <v>92.8</v>
       </c>
-      <c r="D56" s="3">
+      <c r="D56" s="5">
         <v>91.2</v>
       </c>
     </row>
@@ -1311,7 +1320,7 @@
       <c r="C57">
         <v>92.8</v>
       </c>
-      <c r="D57" s="3">
+      <c r="D57" s="5">
         <v>91.2</v>
       </c>
     </row>
@@ -1325,7 +1334,7 @@
       <c r="C58">
         <v>92.8</v>
       </c>
-      <c r="D58" s="3">
+      <c r="D58" s="5">
         <v>91.2</v>
       </c>
     </row>
@@ -1339,7 +1348,7 @@
       <c r="C59">
         <v>92.8</v>
       </c>
-      <c r="D59" s="3">
+      <c r="D59" s="5">
         <v>91.2</v>
       </c>
     </row>
@@ -1353,7 +1362,7 @@
       <c r="C60">
         <v>93.8</v>
       </c>
-      <c r="D60" s="3">
+      <c r="D60" s="5">
         <v>92.4</v>
       </c>
     </row>
@@ -1367,7 +1376,7 @@
       <c r="C61">
         <v>93.8</v>
       </c>
-      <c r="D61" s="3">
+      <c r="D61" s="5">
         <v>92.4</v>
       </c>
     </row>
@@ -1381,7 +1390,7 @@
       <c r="C62">
         <v>93.8</v>
       </c>
-      <c r="D62" s="3">
+      <c r="D62" s="5">
         <v>92.4</v>
       </c>
     </row>
@@ -1395,7 +1404,7 @@
       <c r="C63">
         <v>93.8</v>
       </c>
-      <c r="D63" s="3">
+      <c r="D63" s="5">
         <v>92.4</v>
       </c>
     </row>
@@ -1409,7 +1418,7 @@
       <c r="C64">
         <v>93.8</v>
       </c>
-      <c r="D64" s="3">
+      <c r="D64" s="5">
         <v>92.4</v>
       </c>
     </row>
@@ -1423,7 +1432,7 @@
       <c r="C65">
         <v>93.8</v>
       </c>
-      <c r="D65" s="3">
+      <c r="D65" s="5">
         <v>92.4</v>
       </c>
     </row>
@@ -1437,7 +1446,7 @@
       <c r="C66">
         <v>93.8</v>
       </c>
-      <c r="D66" s="3">
+      <c r="D66" s="5">
         <v>92.4</v>
       </c>
     </row>
@@ -1451,7 +1460,7 @@
       <c r="C67">
         <v>93.8</v>
       </c>
-      <c r="D67" s="3">
+      <c r="D67" s="5">
         <v>92.4</v>
       </c>
     </row>
@@ -1465,7 +1474,7 @@
       <c r="C68">
         <v>93.8</v>
       </c>
-      <c r="D68" s="3">
+      <c r="D68" s="5">
         <v>92.4</v>
       </c>
     </row>
@@ -1479,7 +1488,7 @@
       <c r="C69">
         <v>93.8</v>
       </c>
-      <c r="D69" s="3">
+      <c r="D69" s="5">
         <v>92.4</v>
       </c>
     </row>
@@ -1493,7 +1502,7 @@
       <c r="C70">
         <v>89.4</v>
       </c>
-      <c r="D70" s="3">
+      <c r="D70" s="5">
         <v>83</v>
       </c>
     </row>
@@ -1507,7 +1516,7 @@
       <c r="C71">
         <v>89.4</v>
       </c>
-      <c r="D71" s="3">
+      <c r="D71" s="5">
         <v>83</v>
       </c>
     </row>
@@ -1521,7 +1530,7 @@
       <c r="C72">
         <v>89.4</v>
       </c>
-      <c r="D72" s="3">
+      <c r="D72" s="5">
         <v>83</v>
       </c>
     </row>
@@ -1535,7 +1544,7 @@
       <c r="C73">
         <v>89.4</v>
       </c>
-      <c r="D73" s="3">
+      <c r="D73" s="5">
         <v>83</v>
       </c>
     </row>
@@ -1549,7 +1558,7 @@
       <c r="C74">
         <v>89.4</v>
       </c>
-      <c r="D74" s="3">
+      <c r="D74" s="5">
         <v>83</v>
       </c>
     </row>
@@ -1563,7 +1572,7 @@
       <c r="C75">
         <v>89.4</v>
       </c>
-      <c r="D75" s="3">
+      <c r="D75" s="5">
         <v>83</v>
       </c>
     </row>
@@ -1577,7 +1586,7 @@
       <c r="C76">
         <v>89.4</v>
       </c>
-      <c r="D76" s="3">
+      <c r="D76" s="5">
         <v>83</v>
       </c>
     </row>
@@ -1591,7 +1600,7 @@
       <c r="C77">
         <v>89.4</v>
       </c>
-      <c r="D77" s="3">
+      <c r="D77" s="5">
         <v>83</v>
       </c>
     </row>
@@ -1605,7 +1614,7 @@
       <c r="C78">
         <v>89.4</v>
       </c>
-      <c r="D78" s="3">
+      <c r="D78" s="5">
         <v>83</v>
       </c>
     </row>
@@ -1619,7 +1628,7 @@
       <c r="C79">
         <v>89.4</v>
       </c>
-      <c r="D79" s="3">
+      <c r="D79" s="5">
         <v>83</v>
       </c>
     </row>
@@ -1633,7 +1642,7 @@
       <c r="C80">
         <v>65.7</v>
       </c>
-      <c r="D80" s="3">
+      <c r="D80" s="5">
         <v>70.3</v>
       </c>
     </row>
@@ -1647,7 +1656,7 @@
       <c r="C81">
         <v>65.7</v>
       </c>
-      <c r="D81" s="3">
+      <c r="D81" s="5">
         <v>70.3</v>
       </c>
     </row>
@@ -1661,7 +1670,7 @@
       <c r="C82">
         <v>65.7</v>
       </c>
-      <c r="D82" s="3">
+      <c r="D82" s="5">
         <v>70.3</v>
       </c>
     </row>
@@ -1675,7 +1684,7 @@
       <c r="C83">
         <v>65.7</v>
       </c>
-      <c r="D83" s="3">
+      <c r="D83" s="5">
         <v>70.3</v>
       </c>
     </row>
@@ -1689,7 +1698,7 @@
       <c r="C84">
         <v>65.7</v>
       </c>
-      <c r="D84" s="3">
+      <c r="D84" s="5">
         <v>70.3</v>
       </c>
     </row>
@@ -1703,7 +1712,7 @@
       <c r="C85">
         <v>65.7</v>
       </c>
-      <c r="D85" s="3">
+      <c r="D85" s="5">
         <v>70.3</v>
       </c>
     </row>
@@ -1717,7 +1726,7 @@
       <c r="C86">
         <v>65.7</v>
       </c>
-      <c r="D86" s="3">
+      <c r="D86" s="5">
         <v>70.3</v>
       </c>
     </row>
@@ -1731,7 +1740,7 @@
       <c r="C87">
         <v>65.7</v>
       </c>
-      <c r="D87" s="3">
+      <c r="D87" s="5">
         <v>70.3</v>
       </c>
     </row>
@@ -1745,7 +1754,7 @@
       <c r="C88">
         <v>65.7</v>
       </c>
-      <c r="D88" s="3">
+      <c r="D88" s="5">
         <v>70.3</v>
       </c>
     </row>
@@ -1759,7 +1768,7 @@
       <c r="C89">
         <v>65.7</v>
       </c>
-      <c r="D89" s="3">
+      <c r="D89" s="5">
         <v>70.3</v>
       </c>
     </row>
@@ -1773,7 +1782,7 @@
       <c r="C90">
         <v>65.7</v>
       </c>
-      <c r="D90" s="3">
+      <c r="D90" s="5">
         <v>70.3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Cleaned up a little
</commit_message>
<xml_diff>
--- a/Exel_datasheet.xlsx
+++ b/Exel_datasheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Hugo/Documents/GitHub/Cancer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E6E68F6-48C1-924F-A286-02D18FBA1B47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B86A2FAB-D430-D54A-BCB1-012DE13F3E39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="500" windowWidth="20120" windowHeight="14420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17600" yWindow="5500" windowWidth="20120" windowHeight="14420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -457,7 +457,7 @@
   <dimension ref="A1:H90"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Adding country specific data
</commit_message>
<xml_diff>
--- a/Exel_datasheet.xlsx
+++ b/Exel_datasheet.xlsx
@@ -8,14 +8,27 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Hugo/Documents/GitHub/Cancer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B86A2FAB-D430-D54A-BCB1-012DE13F3E39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8E5ECD8-728B-9D44-9484-921B942B7996}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="17600" yWindow="5500" windowWidth="20120" windowHeight="14420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -457,13 +470,13 @@
   <dimension ref="A1:H90"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="E86" sqref="E86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="30.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="37.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.5" style="5" customWidth="1"/>
     <col min="3" max="3" width="13" style="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13" style="9" bestFit="1" customWidth="1"/>
     <col min="5" max="8" width="13" bestFit="1" customWidth="1"/>

</xml_diff>